<commit_message>
Grading Strategy Testing and add single test suite
</commit_message>
<xml_diff>
--- a/excel/TestSuiteSubmission.xlsx
+++ b/excel/TestSuiteSubmission.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Notes\AutoGraderProject\pysheetgrader-core\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B066C02A-DCE7-43EA-8595-9475D694EE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0641E4D4-5A11-4217-A63E-E79DC3EC1763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{25829142-FE91-0A44-A382-25CA1666B681}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="3" activeTab="7" xr2:uid="{25829142-FE91-0A44-A382-25CA1666B681}"/>
   </bookViews>
   <sheets>
-    <sheet name="SoftFormula Samples" sheetId="9" r:id="rId1"/>
+    <sheet name="Check Samples" sheetId="5" r:id="rId1"/>
     <sheet name="Constant Samples" sheetId="1" r:id="rId2"/>
-    <sheet name="Relative Samples" sheetId="8" r:id="rId3"/>
-    <sheet name="Formula Samples" sheetId="2" r:id="rId4"/>
+    <sheet name="Formula Samples" sheetId="2" r:id="rId3"/>
+    <sheet name="Relative Samples" sheetId="8" r:id="rId4"/>
     <sheet name="RelativeF Samples" sheetId="6" r:id="rId5"/>
-    <sheet name="Check Samples" sheetId="5" r:id="rId6"/>
+    <sheet name="SoftFormula Samples" sheetId="9" r:id="rId6"/>
     <sheet name="Test Case Samples" sheetId="7" r:id="rId7"/>
+    <sheet name="Minimum Work" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
   <si>
     <t>Sample Data</t>
   </si>
@@ -72,15 +73,9 @@
     <t xml:space="preserve"> &gt; This cell is purposefully filled with wrong answer.</t>
   </si>
   <si>
-    <t>&gt; This will be considered as correct due to the delta.</t>
-  </si>
-  <si>
     <t>&gt; This will be considered as correct due to the alt_cells.</t>
   </si>
   <si>
-    <t>&gt; This cell is purposefully filled with wrong answer.</t>
-  </si>
-  <si>
     <t>&gt; This cell will be considered as wrong because it inputs a constant value, not a formula.</t>
   </si>
   <si>
@@ -115,6 +110,51 @@
   </si>
   <si>
     <t>Century Rounder</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Pre-req failure</t>
+  </si>
+  <si>
+    <t>delta correct</t>
+  </si>
+  <si>
+    <t>alt cell correct</t>
+  </si>
+  <si>
+    <t>Bad Mistake</t>
+  </si>
+  <si>
+    <t>No Mistake</t>
+  </si>
+  <si>
+    <t>Negative Grade True</t>
+  </si>
+  <si>
+    <t>Negative Grade False</t>
+  </si>
+  <si>
+    <t>One More</t>
+  </si>
+  <si>
+    <t>pre-req wrong</t>
+  </si>
+  <si>
+    <t>pre-req right</t>
+  </si>
+  <si>
+    <t>&gt; Correct</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>No formula</t>
+  </si>
+  <si>
+    <t>Deliberately wrong</t>
   </si>
 </sst>
 </file>
@@ -475,138 +515,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45F00BE-C631-442C-8DA0-AE0749BE8D75}">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE26CD8-B5F9-2843-9F16-9C9C6D979FA1}">
+  <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="8.796875" style="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>202</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <f>ROUNDUP(B2 * 0.01, 0)</f>
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="C6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <f>B6 * 0.001</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <f>B6 * 3.28</f>
-        <v>3280</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <f>B6*39.37</f>
-        <v>39370</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="1">
-        <f>B2+B3+B4</f>
-        <v>2243</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="1">
-        <f>B2+B3+B4+4-2</f>
-        <v>2245</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF32E925-6E02-734C-B233-A410012DB67F}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -630,6 +609,9 @@
       <c r="B2">
         <v>2020</v>
       </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -638,6 +620,9 @@
       <c r="B3">
         <v>200</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -647,7 +632,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -655,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1200</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -663,10 +648,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -677,7 +659,7 @@
         <v>3281</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -688,7 +670,23 @@
         <v>39370</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -697,84 +695,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B156675-45F5-4D88-8EF2-C0EA21B021CF}">
-  <dimension ref="A2:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E54FCC73-D8ED-7C43-AC38-2299ABF8D40E}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>3003</v>
-      </c>
-      <c r="B2">
-        <v>1001</v>
-      </c>
-      <c r="C2">
-        <v>2002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>4005</v>
-      </c>
-      <c r="B3">
-        <v>2002</v>
-      </c>
-      <c r="C3">
-        <v>2002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3005</v>
-      </c>
-      <c r="B4">
-        <v>1000</v>
-      </c>
-      <c r="C4">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>8888</v>
-      </c>
-      <c r="B5">
-        <v>1000</v>
-      </c>
-      <c r="C5">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2000</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6">
-        <v>1000</v>
-      </c>
-      <c r="D6">
-        <v>2000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E54FCC73-D8ED-7C43-AC38-2299ABF8D40E}">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -807,7 +732,7 @@
         <v>200</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -819,7 +744,7 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -838,6 +763,9 @@
         <f xml:space="preserve"> B6 * 0.001</f>
         <v>1</v>
       </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -848,7 +776,7 @@
         <v>3280</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -860,31 +788,181 @@
         <v>39370</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B11">
+        <f>B2/1000</f>
+        <v>4.04</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
         <f>B2+B3+B4</f>
         <v>4281</v>
       </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12">
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
         <f>B2+B3+B4+4-2</f>
         <v>4283</v>
       </c>
-      <c r="C12" t="s">
-        <v>19</v>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <f>B2/5</f>
+        <v>808</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <f>B2/8</f>
+        <v>505</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B156675-45F5-4D88-8EF2-C0EA21B021CF}">
+  <dimension ref="A2:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>3003</v>
+      </c>
+      <c r="B2">
+        <v>1001</v>
+      </c>
+      <c r="C2">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>4005</v>
+      </c>
+      <c r="B3">
+        <v>2002</v>
+      </c>
+      <c r="C3">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3005</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8888</v>
+      </c>
+      <c r="B5">
+        <v>1000</v>
+      </c>
+      <c r="C5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3000</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3000</v>
+      </c>
+      <c r="B7">
+        <v>1000</v>
+      </c>
+      <c r="C7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3000</v>
+      </c>
+      <c r="B8">
+        <v>1000</v>
+      </c>
+      <c r="C8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2000</v>
+      </c>
+      <c r="B9">
+        <v>1000</v>
+      </c>
+      <c r="C9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2000</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+      <c r="D10">
+        <v>2000</v>
+      </c>
+      <c r="F10">
+        <v>3000</v>
       </c>
     </row>
   </sheetData>
@@ -894,10 +972,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA248177-445A-4F41-8DB3-B508896FF9D2}">
-  <dimension ref="A2:F6"/>
+  <dimension ref="A2:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -905,7 +983,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>E2-F2</f>
-        <v>3099</v>
+        <v>3003</v>
       </c>
       <c r="B2">
         <v>1001</v>
@@ -914,7 +992,7 @@
         <v>2002</v>
       </c>
       <c r="E2">
-        <v>4100</v>
+        <v>4004</v>
       </c>
       <c r="F2">
         <v>1001</v>
@@ -976,16 +1054,73 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
+        <f>E6+F6</f>
+        <v>3005</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6">
         <v>2000</v>
       </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6">
-        <v>1000</v>
-      </c>
-      <c r="D6">
+      <c r="E6">
+        <v>1000</v>
+      </c>
+      <c r="F6">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f>E7+F7</f>
+        <v>3005</v>
+      </c>
+      <c r="B7">
+        <v>1000</v>
+      </c>
+      <c r="C7">
         <v>2000</v>
+      </c>
+      <c r="E7">
+        <v>1000</v>
+      </c>
+      <c r="F7">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3005</v>
+      </c>
+      <c r="B8">
+        <v>1000</v>
+      </c>
+      <c r="C8">
+        <v>2000</v>
+      </c>
+      <c r="E8">
+        <v>1000</v>
+      </c>
+      <c r="F8">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f>E9+F9</f>
+        <v>4005</v>
+      </c>
+      <c r="B9">
+        <v>2002</v>
+      </c>
+      <c r="C9">
+        <v>2002</v>
+      </c>
+      <c r="E9">
+        <v>1000</v>
+      </c>
+      <c r="F9">
+        <v>3005</v>
       </c>
     </row>
   </sheetData>
@@ -994,77 +1129,149 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE26CD8-B5F9-2843-9F16-9C9C6D979FA1}">
-  <dimension ref="B2:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45F00BE-C631-442C-8DA0-AE0749BE8D75}">
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2">
-        <v>50</v>
-      </c>
-      <c r="C2">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="B2" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>202</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <f>ROUNDUP(B2 * 0.01, 0)</f>
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <f>B6 * 0.001</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
+      <c r="B8" s="1">
+        <f>B6 * 3.28</f>
+        <v>3280</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <f>B6*39.37</f>
+        <v>39370</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>6</v>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <f>B2+B3+B4</f>
+        <v>2243</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1">
+        <f>B2+B3+B4+4-2</f>
+        <v>2245</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2243</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F66203-56DE-4670-B232-2142CFFE2447}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1097,12 +1304,12 @@
         <v>202</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1117,7 +1324,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1146,7 +1353,7 @@
         <v>3281</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1158,7 +1365,133 @@
         <v>39370</v>
       </c>
       <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <f>B7*39.37</f>
+        <v>39370</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2940D7-F028-41AF-9DCC-CB6DDE1DE7F0}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.296875" customWidth="1"/>
+    <col min="2" max="2" width="13.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2020</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3281</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>39370</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes for check rubric
</commit_message>
<xml_diff>
--- a/excel/TestSuiteSubmission.xlsx
+++ b/excel/TestSuiteSubmission.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Notes\AutoGraderProject\pysheetgrader-core\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4801220-F491-4451-BF15-3C07A83E5DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CAD94F-15BC-4BFA-8D12-B40E4A23C05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50415" yWindow="8370" windowWidth="11070" windowHeight="6030" firstSheet="4" activeTab="5" xr2:uid="{25829142-FE91-0A44-A382-25CA1666B681}"/>
+    <workbookView xWindow="0" yWindow="6432" windowWidth="8856" windowHeight="4836" firstSheet="2" activeTab="2" xr2:uid="{25829142-FE91-0A44-A382-25CA1666B681}"/>
   </bookViews>
   <sheets>
-    <sheet name="Check Samples" sheetId="5" r:id="rId1"/>
-    <sheet name="Constant Samples" sheetId="1" r:id="rId2"/>
-    <sheet name="Formula Samples" sheetId="2" r:id="rId3"/>
-    <sheet name="Relative Samples" sheetId="8" r:id="rId4"/>
-    <sheet name="RelativeF Samples" sheetId="6" r:id="rId5"/>
-    <sheet name="SoftFormula Samples" sheetId="9" r:id="rId6"/>
+    <sheet name="Relative Samples" sheetId="8" r:id="rId1"/>
+    <sheet name="SoftFormula Samples" sheetId="9" r:id="rId2"/>
+    <sheet name="Check Samples" sheetId="5" r:id="rId3"/>
+    <sheet name="Constant Samples" sheetId="1" r:id="rId4"/>
+    <sheet name="Formula Samples" sheetId="2" r:id="rId5"/>
+    <sheet name="RelativeF Samples" sheetId="6" r:id="rId6"/>
     <sheet name="Test Case Samples" sheetId="7" r:id="rId7"/>
     <sheet name="Minimum Work" sheetId="10" r:id="rId8"/>
   </sheets>
@@ -524,11 +524,269 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE26CD8-B5F9-2843-9F16-9C9C6D979FA1}">
-  <dimension ref="B2:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B156675-45F5-4D88-8EF2-C0EA21B021CF}">
+  <dimension ref="A2:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>3003</v>
+      </c>
+      <c r="B2">
+        <v>1001</v>
+      </c>
+      <c r="C2">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>4005</v>
+      </c>
+      <c r="B3">
+        <v>2002</v>
+      </c>
+      <c r="C3">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3005</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8888</v>
+      </c>
+      <c r="B5">
+        <v>1000</v>
+      </c>
+      <c r="C5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3000</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3000</v>
+      </c>
+      <c r="B7">
+        <v>1000</v>
+      </c>
+      <c r="C7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3000</v>
+      </c>
+      <c r="B8">
+        <v>1000</v>
+      </c>
+      <c r="C8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2000</v>
+      </c>
+      <c r="B9">
+        <v>1000</v>
+      </c>
+      <c r="C9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2000</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+      <c r="D10">
+        <v>2000</v>
+      </c>
+      <c r="F10">
+        <v>3000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45F00BE-C631-442C-8DA0-AE0749BE8D75}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>202</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <f>ROUNDUP(B2 * 0.01, 0)</f>
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <f>B6 * 0.001</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <f>B6 * 3.28</f>
+        <v>3280</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <f>B6*39.37</f>
+        <v>39370</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <f>B2+B3+B4</f>
+        <v>2243</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <f>B2+B3+B4+4-2</f>
+        <v>2245</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2243</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE26CD8-B5F9-2843-9F16-9C9C6D979FA1}">
+  <dimension ref="B2:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -576,12 +834,52 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -589,7 +887,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF32E925-6E02-734C-B233-A410012DB67F}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -709,7 +1007,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E54FCC73-D8ED-7C43-AC38-2299ABF8D40E}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -865,127 +1163,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B156675-45F5-4D88-8EF2-C0EA21B021CF}">
-  <dimension ref="A2:F10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>3003</v>
-      </c>
-      <c r="B2">
-        <v>1001</v>
-      </c>
-      <c r="C2">
-        <v>2002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>4005</v>
-      </c>
-      <c r="B3">
-        <v>2002</v>
-      </c>
-      <c r="C3">
-        <v>2002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3005</v>
-      </c>
-      <c r="B4">
-        <v>1000</v>
-      </c>
-      <c r="C4">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>8888</v>
-      </c>
-      <c r="B5">
-        <v>1000</v>
-      </c>
-      <c r="C5">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>3000</v>
-      </c>
-      <c r="B6">
-        <v>1000</v>
-      </c>
-      <c r="C6">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>3000</v>
-      </c>
-      <c r="B7">
-        <v>1000</v>
-      </c>
-      <c r="C7">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>3000</v>
-      </c>
-      <c r="B8">
-        <v>1000</v>
-      </c>
-      <c r="C8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2000</v>
-      </c>
-      <c r="B9">
-        <v>1000</v>
-      </c>
-      <c r="C9">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2000</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>1000</v>
-      </c>
-      <c r="D10">
-        <v>2000</v>
-      </c>
-      <c r="F10">
-        <v>3000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA248177-445A-4F41-8DB3-B508896FF9D2}">
   <dimension ref="A2:F9"/>
   <sheetViews>
@@ -1140,144 +1318,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45F00BE-C631-442C-8DA0-AE0749BE8D75}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="8.796875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>202</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <f>ROUNDUP(B2 * 0.01, 0)</f>
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <f>B6 * 0.001</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <f>B6 * 3.28</f>
-        <v>3280</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <f>B6*39.37</f>
-        <v>39370</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1">
-        <f>B2+B3+B4</f>
-        <v>2243</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1">
-        <f>B2+B3+B4+4-2</f>
-        <v>2245</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="1">
-        <v>2243</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>